<commit_message>
Added SQL export files for creating tables
</commit_message>
<xml_diff>
--- a/Coursework/Normalisation.xlsx
+++ b/Coursework/Normalisation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="129">
   <si>
     <t>UNF</t>
   </si>
@@ -322,9 +322,6 @@
     <t>Table</t>
   </si>
   <si>
-    <t>Datetime</t>
-  </si>
-  <si>
     <t>DD/MM/YYYY</t>
   </si>
   <si>
@@ -392,6 +389,18 @@
   </si>
   <si>
     <t>buttery, flaky pastry</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -818,16 +827,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G190" sqref="G190"/>
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G184" sqref="G184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="7" width="27.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
+    <col min="2" max="9" width="30.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="33.85546875" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -2928,7 +2935,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B177" s="1" t="s">
         <v>15</v>
       </c>
@@ -2939,7 +2946,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B178" s="1" t="s">
         <v>14</v>
       </c>
@@ -2953,7 +2960,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B179" s="1" t="s">
         <v>13</v>
       </c>
@@ -2964,7 +2971,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B180" s="1" t="s">
         <v>16</v>
       </c>
@@ -2975,7 +2982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C181" s="1" t="s">
         <v>14</v>
       </c>
@@ -2989,7 +2996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C182" s="1" t="s">
         <v>13</v>
       </c>
@@ -3000,7 +3007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C183" s="1" t="s">
         <v>16</v>
       </c>
@@ -3011,7 +3018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D184" s="1" t="s">
         <v>13</v>
       </c>
@@ -3019,7 +3026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D185" s="1" t="s">
         <v>16</v>
       </c>
@@ -3028,15 +3035,15 @@
       </c>
       <c r="F185" s="3"/>
     </row>
-    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E186" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F187" s="3"/>
     </row>
-    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B189" s="1" t="s">
         <v>87</v>
       </c>
@@ -3044,14 +3051,14 @@
       <c r="E189" s="2"/>
       <c r="F189" s="3"/>
     </row>
-    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E190" s="2"/>
       <c r="F190" s="3"/>
     </row>
-    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C191" s="2"/>
     </row>
-    <row r="192" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B192" s="7" t="s">
         <v>101</v>
       </c>
@@ -3065,16 +3072,19 @@
         <v>88</v>
       </c>
       <c r="F192" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G192" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G192" s="8" t="s">
+      <c r="H192" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H192" s="8" t="s">
+      <c r="I192" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="193" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B193" s="9" t="s">
         <v>44</v>
       </c>
@@ -3085,19 +3095,22 @@
         <v>92</v>
       </c>
       <c r="E193" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F193" s="10">
+        <v>107</v>
+      </c>
+      <c r="F193" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G193" s="10">
         <v>5</v>
       </c>
-      <c r="G193" s="9" t="s">
+      <c r="H193" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="H193" s="10">
+      <c r="I193" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B194" s="9"/>
       <c r="C194" s="9" t="s">
         <v>79</v>
@@ -3106,17 +3119,20 @@
         <v>93</v>
       </c>
       <c r="E194" s="10"/>
-      <c r="F194" s="10">
+      <c r="F194" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G194" s="10">
         <v>20</v>
       </c>
-      <c r="G194" s="9" t="s">
+      <c r="H194" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H194" s="10" t="s">
+      <c r="I194" s="10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="195" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B195" s="9"/>
       <c r="C195" s="9" t="s">
         <v>99</v>
@@ -3125,17 +3141,20 @@
         <v>93</v>
       </c>
       <c r="E195" s="10"/>
-      <c r="F195" s="10">
+      <c r="F195" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G195" s="10">
         <v>20</v>
       </c>
-      <c r="G195" s="9" t="s">
+      <c r="H195" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="H195" s="10" t="s">
+      <c r="I195" s="10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="196" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B196" s="9" t="s">
         <v>35</v>
       </c>
@@ -3146,61 +3165,70 @@
         <v>92</v>
       </c>
       <c r="E196" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F196" s="10">
+        <v>107</v>
+      </c>
+      <c r="F196" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G196" s="10">
         <v>5</v>
       </c>
-      <c r="G196" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H196" s="10">
+      <c r="H196" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I196" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B197" s="9"/>
       <c r="C197" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D197" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E197" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E197" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F197" s="10">
+      <c r="F197" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G197" s="10">
         <v>10</v>
       </c>
-      <c r="G197" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H197" s="12">
+      <c r="H197" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I197" s="12">
         <v>43575</v>
       </c>
     </row>
-    <row r="198" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B198" s="9"/>
       <c r="C198" s="9" t="s">
         <v>81</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E198" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F198" s="10">
+        <v>108</v>
+      </c>
+      <c r="F198" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G198" s="10">
         <v>5</v>
       </c>
-      <c r="G198" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H198" s="10">
+      <c r="H198" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I198" s="10">
         <v>13.99</v>
       </c>
     </row>
-    <row r="199" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B199" s="9" t="s">
         <v>37</v>
       </c>
@@ -3211,40 +3239,46 @@
         <v>92</v>
       </c>
       <c r="E199" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F199" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G199" s="10">
+        <v>2</v>
+      </c>
+      <c r="H199" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F199" s="10">
-        <v>2</v>
-      </c>
-      <c r="G199" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="H199" s="10">
+      <c r="I199" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B200" s="9"/>
       <c r="C200" s="9" t="s">
         <v>80</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E200" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F200" s="10">
+        <v>108</v>
+      </c>
+      <c r="F200" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G200" s="10">
         <v>5</v>
       </c>
-      <c r="G200" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H200" s="10">
+      <c r="H200" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I200" s="10">
         <v>5.99</v>
       </c>
     </row>
-    <row r="201" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B201" s="9" t="s">
         <v>34</v>
       </c>
@@ -3255,61 +3289,70 @@
         <v>92</v>
       </c>
       <c r="E201" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F201" s="10">
+        <v>107</v>
+      </c>
+      <c r="F201" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G201" s="10">
         <v>5</v>
       </c>
-      <c r="G201" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H201" s="10">
+      <c r="H201" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I201" s="10">
         <v>6</v>
       </c>
     </row>
-    <row r="202" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B202" s="9"/>
       <c r="C202" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D202" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E202" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E202" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F202" s="10">
+      <c r="F202" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G202" s="10">
         <v>5</v>
       </c>
-      <c r="G202" s="9" t="s">
+      <c r="H202" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="I202" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="H202" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="203" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="203" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B203" s="9"/>
       <c r="C203" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D203" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E203" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F203" s="10">
+        <v>108</v>
+      </c>
+      <c r="F203" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G203" s="10">
         <v>5</v>
       </c>
-      <c r="G203" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H203" s="10">
+      <c r="H203" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I203" s="10">
         <v>3.55</v>
       </c>
     </row>
-    <row r="204" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B204" s="9"/>
       <c r="C204" s="9" t="s">
         <v>14</v>
@@ -3318,17 +3361,20 @@
         <v>93</v>
       </c>
       <c r="E204" s="10"/>
-      <c r="F204" s="10">
+      <c r="F204" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G204" s="10">
         <v>20</v>
       </c>
-      <c r="G204" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H204" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="205" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="H204" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="I204" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="205" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B205" s="9"/>
       <c r="C205" s="9" t="s">
         <v>13</v>
@@ -3337,33 +3383,39 @@
         <v>92</v>
       </c>
       <c r="E205" s="10"/>
-      <c r="F205" s="10">
+      <c r="F205" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G205" s="10">
         <v>4</v>
       </c>
-      <c r="G205" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="H205" s="10">
+      <c r="H205" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="I205" s="10">
         <v>400</v>
       </c>
     </row>
-    <row r="206" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B206" s="9"/>
       <c r="C206" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D206" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E206" s="10"/>
+      <c r="F206" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G206" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E206" s="10"/>
-      <c r="F206" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="G206" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="H206" s="13" t="s">
-        <v>125</v>
+      <c r="H206" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I206" s="13" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>